<commit_message>
re-organised the layout and made it clearer for readers
</commit_message>
<xml_diff>
--- a/output_changed_stats_by_site.xlsx
+++ b/output_changed_stats_by_site.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="208">
   <si>
     <t>en_name</t>
   </si>
@@ -67,6 +67,12 @@
     <t>Improving -&gt; Stable</t>
   </si>
   <si>
+    <t>Area de Conservación Guanacaste</t>
+  </si>
+  <si>
+    <t>Effective -&gt; Some Concern</t>
+  </si>
+  <si>
     <t>Atlantic Forest Southeast Reserves</t>
   </si>
   <si>
@@ -136,9 +142,6 @@
     <t>Cape Floral Region Protected Areas</t>
   </si>
   <si>
-    <t>Effective -&gt; Some Concern</t>
-  </si>
-  <si>
     <t>Carlsbad Caverns National Park</t>
   </si>
   <si>
@@ -157,6 +160,9 @@
     <t>Good -&gt; Good with some concerns</t>
   </si>
   <si>
+    <t>Central Amazon Conservation Complex</t>
+  </si>
+  <si>
     <t>Central Sikhote-Alin</t>
   </si>
   <si>
@@ -262,6 +268,12 @@
     <t>El Pinacate and Gran Desierto de Altar Biosphere Reserve</t>
   </si>
   <si>
+    <t>Fraser Island</t>
+  </si>
+  <si>
+    <t>Galápagos Islands</t>
+  </si>
+  <si>
     <t>Garamba National Park</t>
   </si>
   <si>
@@ -283,6 +295,9 @@
     <t>Gros Morne National Park</t>
   </si>
   <si>
+    <t>Göreme National Park and the Rock Sites of Cappadocia</t>
+  </si>
+  <si>
     <t>Ha Long Bay</t>
   </si>
   <si>
@@ -295,6 +310,9 @@
     <t>Henderson Island</t>
   </si>
   <si>
+    <t>Hierapolis-Pamukkale</t>
+  </si>
+  <si>
     <t>Historic Sanctuary of Machu Picchu</t>
   </si>
   <si>
@@ -325,6 +343,9 @@
     <t>nan -&gt; Low Threat</t>
   </si>
   <si>
+    <t>Isole Eolie (Aeolian Islands)</t>
+  </si>
+  <si>
     <t>Jeju Volcanic Island and Lava Tubes</t>
   </si>
   <si>
@@ -340,6 +361,9 @@
     <t>Highly Effective -&gt; Effective</t>
   </si>
   <si>
+    <t>Kaziranga National Park</t>
+  </si>
+  <si>
     <t>Keoladeo National Park</t>
   </si>
   <si>
@@ -397,9 +421,24 @@
     <t>Miguasha National Park</t>
   </si>
   <si>
+    <t>Monarch Butterfly Biosphere Reserve</t>
+  </si>
+  <si>
+    <t>Critical -&gt; Data Deficient</t>
+  </si>
+  <si>
     <t>Monte San Giorgio</t>
   </si>
   <si>
+    <t>Mount Etna</t>
+  </si>
+  <si>
+    <t>Stable -&gt; Improving</t>
+  </si>
+  <si>
+    <t>nan -&gt; Very Low Threat</t>
+  </si>
+  <si>
     <t>Mount Hamiguitan Range Wildlife Sanctuary</t>
   </si>
   <si>
@@ -418,6 +457,9 @@
     <t>Nahanni National Park</t>
   </si>
   <si>
+    <t>Nanda Devi and Valley of Flowers National Parks</t>
+  </si>
+  <si>
     <t>Natural and Cultural Heritage of the Ohrid region</t>
   </si>
   <si>
@@ -430,9 +472,6 @@
     <t>Niokolo-Koba National Park</t>
   </si>
   <si>
-    <t>Critical -&gt; Data Deficient</t>
-  </si>
-  <si>
     <t>Ogasawara Islands</t>
   </si>
   <si>
@@ -454,6 +493,9 @@
     <t>Good -&gt; Data Deficient</t>
   </si>
   <si>
+    <t>Phong Nha-Ke Bang National Park</t>
+  </si>
+  <si>
     <t>Pitons, cirques and remparts of Reunion Island</t>
   </si>
   <si>
@@ -469,6 +511,9 @@
     <t>Stable -&gt; nan</t>
   </si>
   <si>
+    <t>Plitvice Lakes National Park</t>
+  </si>
+  <si>
     <t>Puerto-Princesa Subterranean River National Park</t>
   </si>
   <si>
@@ -481,15 +526,15 @@
     <t>Rwenzori Mountains National Park</t>
   </si>
   <si>
+    <t>Río Plátano Biosphere Reserve</t>
+  </si>
+  <si>
     <t>Sangha Trinational</t>
   </si>
   <si>
     <t>Saryarka – Steppe and Lakes of Northern Kazakhstan</t>
   </si>
   <si>
-    <t>Stable -&gt; Improving</t>
-  </si>
-  <si>
     <t>Selous Game Reserve</t>
   </si>
   <si>
@@ -529,6 +574,9 @@
     <t>Tassili n'Ajjer</t>
   </si>
   <si>
+    <t>The Dolomites</t>
+  </si>
+  <si>
     <t>Three Parallel Rivers of Yunnan Protected Areas</t>
   </si>
   <si>
@@ -545,6 +593,9 @@
   </si>
   <si>
     <t>Good with some concerns -&gt; Good</t>
+  </si>
+  <si>
+    <t>Ujung Kulon National Park</t>
   </si>
   <si>
     <t>Uvs Nuur Basin</t>
@@ -935,7 +986,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K112"/>
+  <dimension ref="A1:K128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1009,16 +1060,14 @@
       </c>
       <c r="B3" t="s"/>
       <c r="C3" t="s"/>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
+      <c r="D3" t="s"/>
       <c r="E3" t="s"/>
       <c r="F3" t="s"/>
-      <c r="G3" t="s">
+      <c r="G3" t="s"/>
+      <c r="H3" t="s"/>
+      <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" t="s"/>
-      <c r="I3" t="s"/>
       <c r="J3" t="s"/>
       <c r="K3" t="s"/>
     </row>
@@ -1028,168 +1077,168 @@
       </c>
       <c r="B4" t="s"/>
       <c r="C4" t="s"/>
-      <c r="D4" t="s"/>
-      <c r="E4" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
+      <c r="E4" t="s"/>
       <c r="F4" t="s"/>
-      <c r="G4" t="s"/>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s"/>
+      <c r="I4" t="s"/>
       <c r="J4" t="s"/>
       <c r="K4" t="s"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s"/>
       <c r="C5" t="s"/>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s"/>
+      <c r="D5" t="s"/>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
       <c r="F5" t="s"/>
       <c r="G5" t="s"/>
       <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s"/>
-      <c r="J5" t="s">
-        <v>25</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s"/>
       <c r="K5" t="s"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s"/>
+        <v>25</v>
+      </c>
+      <c r="B6" t="s"/>
+      <c r="C6" t="s"/>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
       <c r="E6" t="s"/>
       <c r="F6" t="s"/>
       <c r="G6" t="s"/>
-      <c r="H6" t="s"/>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
       <c r="I6" t="s"/>
-      <c r="J6" t="s"/>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
       <c r="K6" t="s"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
+      <c r="D7" t="s"/>
       <c r="E7" t="s"/>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
+      <c r="F7" t="s"/>
+      <c r="G7" t="s"/>
       <c r="H7" t="s"/>
-      <c r="I7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" t="s">
-        <v>34</v>
-      </c>
+      <c r="I7" t="s"/>
+      <c r="J7" t="s"/>
+      <c r="K7" t="s"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s"/>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s"/>
+      <c r="I8" t="s">
         <v>35</v>
       </c>
-      <c r="B8" t="s"/>
-      <c r="C8" t="s">
+      <c r="J8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" t="s"/>
-      <c r="F8" t="s"/>
-      <c r="G8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" t="s"/>
-      <c r="J8" t="s"/>
-      <c r="K8" t="s"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s"/>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="B9" t="s"/>
-      <c r="C9" t="s"/>
-      <c r="D9" t="s"/>
       <c r="E9" t="s"/>
-      <c r="F9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" t="s"/>
-      <c r="H9" t="s"/>
-      <c r="I9" t="s">
+      <c r="F9" t="s"/>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
         <v>40</v>
       </c>
-      <c r="J9" t="s">
-        <v>30</v>
-      </c>
+      <c r="I9" t="s"/>
+      <c r="J9" t="s"/>
       <c r="K9" t="s"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
-      </c>
+      <c r="B10" t="s"/>
+      <c r="C10" t="s"/>
       <c r="D10" t="s"/>
       <c r="E10" t="s"/>
-      <c r="F10" t="s"/>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
       <c r="G10" t="s"/>
       <c r="H10" t="s"/>
-      <c r="I10" t="s"/>
-      <c r="J10" t="s"/>
+      <c r="I10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" t="s">
+        <v>32</v>
+      </c>
       <c r="K10" t="s"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
         <v>44</v>
       </c>
-      <c r="B11" t="s"/>
-      <c r="C11" t="s"/>
-      <c r="D11" t="s">
-        <v>45</v>
-      </c>
+      <c r="D11" t="s"/>
       <c r="E11" t="s"/>
-      <c r="F11" t="s">
-        <v>46</v>
-      </c>
+      <c r="F11" t="s"/>
       <c r="G11" t="s"/>
       <c r="H11" t="s"/>
       <c r="I11" t="s"/>
@@ -1198,34 +1247,26 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s"/>
       <c r="C12" t="s"/>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s"/>
       <c r="F12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" t="s">
-        <v>15</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G12" t="s"/>
       <c r="H12" t="s"/>
-      <c r="I12" t="s">
-        <v>49</v>
-      </c>
-      <c r="J12" t="s">
-        <v>50</v>
-      </c>
-      <c r="K12" t="s">
-        <v>43</v>
-      </c>
+      <c r="I12" t="s"/>
+      <c r="J12" t="s"/>
+      <c r="K12" t="s"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s"/>
       <c r="C13" t="s"/>
@@ -1235,293 +1276,297 @@
       <c r="G13" t="s"/>
       <c r="H13" t="s"/>
       <c r="I13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J13" t="s"/>
       <c r="K13" t="s"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s"/>
+      <c r="C14" t="s"/>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s"/>
+      <c r="F14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s"/>
+      <c r="I14" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" t="s">
         <v>52</v>
       </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" t="s"/>
-      <c r="E14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" t="s"/>
-      <c r="G14" t="s"/>
-      <c r="H14" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" t="s"/>
-      <c r="J14" t="s">
-        <v>55</v>
-      </c>
-      <c r="K14" t="s"/>
+      <c r="K14" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s"/>
       <c r="C15" t="s"/>
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
+      <c r="D15" t="s"/>
       <c r="E15" t="s"/>
       <c r="F15" t="s"/>
-      <c r="G15" t="s">
-        <v>37</v>
-      </c>
+      <c r="G15" t="s"/>
       <c r="H15" t="s"/>
-      <c r="I15" t="s"/>
+      <c r="I15" t="s">
+        <v>24</v>
+      </c>
       <c r="J15" t="s"/>
       <c r="K15" t="s"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s"/>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s"/>
+      <c r="G16" t="s"/>
+      <c r="H16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" t="s"/>
+      <c r="J16" t="s">
         <v>57</v>
       </c>
-      <c r="B16" t="s"/>
-      <c r="C16" t="s"/>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" t="s"/>
-      <c r="F16" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16" t="s">
-        <v>60</v>
-      </c>
-      <c r="J16" t="s"/>
-      <c r="K16" t="s">
-        <v>61</v>
-      </c>
+      <c r="K16" t="s"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" t="s"/>
+        <v>58</v>
+      </c>
+      <c r="B17" t="s"/>
+      <c r="C17" t="s"/>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
       <c r="E17" t="s"/>
       <c r="F17" t="s"/>
-      <c r="G17" t="s"/>
-      <c r="H17" t="s">
-        <v>54</v>
-      </c>
+      <c r="G17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" t="s"/>
       <c r="I17" t="s"/>
-      <c r="J17" t="s">
-        <v>64</v>
-      </c>
-      <c r="K17" t="s">
-        <v>65</v>
-      </c>
+      <c r="J17" t="s"/>
+      <c r="K17" t="s"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" t="s"/>
+        <v>59</v>
+      </c>
+      <c r="B18" t="s"/>
+      <c r="C18" t="s"/>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
       <c r="E18" t="s"/>
-      <c r="F18" t="s"/>
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
       <c r="G18" t="s">
-        <v>37</v>
-      </c>
-      <c r="H18" t="s"/>
-      <c r="I18" t="s"/>
+        <v>20</v>
+      </c>
+      <c r="H18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" t="s">
+        <v>62</v>
+      </c>
       <c r="J18" t="s"/>
-      <c r="K18" t="s"/>
+      <c r="K18" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D19" t="s"/>
-      <c r="E19" t="s">
-        <v>14</v>
-      </c>
+      <c r="E19" t="s"/>
       <c r="F19" t="s"/>
       <c r="G19" t="s"/>
-      <c r="H19" t="s"/>
+      <c r="H19" t="s">
+        <v>56</v>
+      </c>
       <c r="I19" t="s"/>
-      <c r="J19" t="s"/>
-      <c r="K19" t="s"/>
+      <c r="J19" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" t="s"/>
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>69</v>
+      </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s"/>
       <c r="E20" t="s"/>
       <c r="F20" t="s"/>
-      <c r="G20" t="s"/>
-      <c r="H20" t="s">
-        <v>72</v>
-      </c>
+      <c r="G20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" t="s"/>
       <c r="I20" t="s"/>
       <c r="J20" t="s"/>
-      <c r="K20" t="s">
-        <v>71</v>
-      </c>
+      <c r="K20" t="s"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" t="s"/>
-      <c r="C21" t="s"/>
-      <c r="D21" t="s">
-        <v>37</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" t="s"/>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F21" t="s"/>
       <c r="G21" t="s"/>
-      <c r="H21" t="s">
-        <v>18</v>
-      </c>
+      <c r="H21" t="s"/>
       <c r="I21" t="s"/>
       <c r="J21" t="s"/>
       <c r="K21" t="s"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" t="s">
-        <v>75</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B22" t="s"/>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s"/>
       <c r="E22" t="s"/>
       <c r="F22" t="s"/>
       <c r="G22" t="s"/>
-      <c r="H22" t="s"/>
+      <c r="H22" t="s">
+        <v>74</v>
+      </c>
       <c r="I22" t="s"/>
       <c r="J22" t="s"/>
-      <c r="K22" t="s"/>
+      <c r="K22" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s"/>
       <c r="C23" t="s"/>
       <c r="D23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" t="s"/>
-      <c r="F23" t="s">
-        <v>58</v>
-      </c>
-      <c r="G23" t="s">
-        <v>18</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s"/>
+      <c r="G23" t="s"/>
       <c r="H23" t="s">
-        <v>21</v>
-      </c>
-      <c r="I23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J23" t="s">
-        <v>25</v>
-      </c>
-      <c r="K23" t="s">
-        <v>61</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I23" t="s"/>
+      <c r="J23" t="s"/>
+      <c r="K23" t="s"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
         <v>78</v>
       </c>
-      <c r="B24" t="s"/>
-      <c r="C24" t="s"/>
       <c r="D24" t="s"/>
       <c r="E24" t="s"/>
       <c r="F24" t="s"/>
       <c r="G24" t="s"/>
-      <c r="H24" t="s">
-        <v>79</v>
-      </c>
+      <c r="H24" t="s"/>
       <c r="I24" t="s"/>
       <c r="J24" t="s"/>
       <c r="K24" t="s"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s"/>
       <c r="C25" t="s"/>
-      <c r="D25" t="s"/>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
       <c r="E25" t="s"/>
       <c r="F25" t="s">
-        <v>58</v>
-      </c>
-      <c r="G25" t="s"/>
-      <c r="H25" t="s"/>
-      <c r="I25" t="s"/>
+        <v>60</v>
+      </c>
+      <c r="G25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" t="s">
+        <v>24</v>
+      </c>
       <c r="J25" t="s">
-        <v>67</v>
-      </c>
-      <c r="K25" t="s"/>
+        <v>27</v>
+      </c>
+      <c r="K25" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s"/>
       <c r="C26" t="s"/>
-      <c r="D26" t="s">
-        <v>24</v>
-      </c>
+      <c r="D26" t="s"/>
       <c r="E26" t="s"/>
-      <c r="F26" t="s">
-        <v>32</v>
-      </c>
+      <c r="F26" t="s"/>
       <c r="G26" t="s"/>
-      <c r="H26" t="s"/>
-      <c r="I26" t="s">
-        <v>40</v>
-      </c>
+      <c r="H26" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" t="s"/>
       <c r="J26" t="s"/>
       <c r="K26" t="s"/>
     </row>
@@ -1533,13 +1578,15 @@
       <c r="C27" t="s"/>
       <c r="D27" t="s"/>
       <c r="E27" t="s"/>
-      <c r="F27" t="s"/>
+      <c r="F27" t="s">
+        <v>60</v>
+      </c>
       <c r="G27" t="s"/>
-      <c r="H27" t="s">
-        <v>24</v>
-      </c>
+      <c r="H27" t="s"/>
       <c r="I27" t="s"/>
-      <c r="J27" t="s"/>
+      <c r="J27" t="s">
+        <v>69</v>
+      </c>
       <c r="K27" t="s"/>
     </row>
     <row r="28" spans="1:11">
@@ -1548,32 +1595,34 @@
       </c>
       <c r="B28" t="s"/>
       <c r="C28" t="s"/>
-      <c r="D28" t="s"/>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
       <c r="E28" t="s"/>
-      <c r="F28" t="s"/>
+      <c r="F28" t="s">
+        <v>34</v>
+      </c>
       <c r="G28" t="s"/>
       <c r="H28" t="s"/>
-      <c r="I28" t="s"/>
-      <c r="J28" t="s">
-        <v>50</v>
-      </c>
+      <c r="I28" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" t="s"/>
       <c r="K28" t="s"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B29" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" t="s">
-        <v>65</v>
-      </c>
+      <c r="B29" t="s"/>
+      <c r="C29" t="s"/>
       <c r="D29" t="s"/>
       <c r="E29" t="s"/>
       <c r="F29" t="s"/>
       <c r="G29" t="s"/>
-      <c r="H29" t="s"/>
+      <c r="H29" t="s">
+        <v>39</v>
+      </c>
       <c r="I29" t="s"/>
       <c r="J29" t="s"/>
       <c r="K29" t="s"/>
@@ -1584,16 +1633,14 @@
       </c>
       <c r="B30" t="s"/>
       <c r="C30" t="s"/>
-      <c r="D30" t="s">
-        <v>37</v>
-      </c>
+      <c r="D30" t="s"/>
       <c r="E30" t="s"/>
       <c r="F30" t="s"/>
       <c r="G30" t="s"/>
-      <c r="H30" t="s"/>
-      <c r="I30" t="s">
-        <v>40</v>
-      </c>
+      <c r="H30" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" t="s"/>
       <c r="J30" t="s"/>
       <c r="K30" t="s"/>
     </row>
@@ -1607,11 +1654,11 @@
       <c r="E31" t="s"/>
       <c r="F31" t="s"/>
       <c r="G31" t="s"/>
-      <c r="H31" t="s"/>
+      <c r="H31" t="s">
+        <v>26</v>
+      </c>
       <c r="I31" t="s"/>
-      <c r="J31" t="s">
-        <v>25</v>
-      </c>
+      <c r="J31" t="s"/>
       <c r="K31" t="s"/>
     </row>
     <row r="32" spans="1:11">
@@ -1624,11 +1671,11 @@
       <c r="E32" t="s"/>
       <c r="F32" t="s"/>
       <c r="G32" t="s"/>
-      <c r="H32" t="s">
-        <v>15</v>
-      </c>
+      <c r="H32" t="s"/>
       <c r="I32" t="s"/>
-      <c r="J32" t="s"/>
+      <c r="J32" t="s">
+        <v>52</v>
+      </c>
       <c r="K32" t="s"/>
     </row>
     <row r="33" spans="1:11">
@@ -1636,17 +1683,17 @@
         <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" t="s"/>
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
       <c r="D33" t="s"/>
       <c r="E33" t="s"/>
       <c r="F33" t="s"/>
       <c r="G33" t="s"/>
       <c r="H33" t="s"/>
-      <c r="I33" t="s">
-        <v>40</v>
-      </c>
+      <c r="I33" t="s"/>
       <c r="J33" t="s"/>
       <c r="K33" t="s"/>
     </row>
@@ -1656,20 +1703,22 @@
       </c>
       <c r="B34" t="s"/>
       <c r="C34" t="s"/>
-      <c r="D34" t="s"/>
+      <c r="D34" t="s">
+        <v>39</v>
+      </c>
       <c r="E34" t="s"/>
       <c r="F34" t="s"/>
       <c r="G34" t="s"/>
       <c r="H34" t="s"/>
-      <c r="I34" t="s"/>
+      <c r="I34" t="s">
+        <v>18</v>
+      </c>
       <c r="J34" t="s"/>
-      <c r="K34" t="s">
-        <v>90</v>
-      </c>
+      <c r="K34" t="s"/>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" t="s"/>
       <c r="C35" t="s"/>
@@ -1680,13 +1729,13 @@
       <c r="H35" t="s"/>
       <c r="I35" t="s"/>
       <c r="J35" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K35" t="s"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s"/>
       <c r="C36" t="s"/>
@@ -1694,37 +1743,35 @@
       <c r="E36" t="s"/>
       <c r="F36" t="s"/>
       <c r="G36" t="s"/>
-      <c r="H36" t="s"/>
-      <c r="I36" t="s">
-        <v>40</v>
-      </c>
+      <c r="H36" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" t="s"/>
       <c r="J36" t="s"/>
       <c r="K36" t="s"/>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>94</v>
-      </c>
-      <c r="C37" t="s">
-        <v>53</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C37" t="s"/>
       <c r="D37" t="s"/>
-      <c r="E37" t="s">
-        <v>14</v>
-      </c>
+      <c r="E37" t="s"/>
       <c r="F37" t="s"/>
       <c r="G37" t="s"/>
       <c r="H37" t="s"/>
-      <c r="I37" t="s"/>
+      <c r="I37" t="s">
+        <v>18</v>
+      </c>
       <c r="J37" t="s"/>
       <c r="K37" t="s"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B38" t="s"/>
       <c r="C38" t="s"/>
@@ -1734,117 +1781,109 @@
       <c r="G38" t="s"/>
       <c r="H38" t="s"/>
       <c r="I38" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="J38" t="s"/>
       <c r="K38" t="s"/>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B39" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" t="s">
-        <v>69</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B39" t="s"/>
+      <c r="C39" t="s"/>
       <c r="D39" t="s"/>
-      <c r="E39" t="s">
-        <v>97</v>
-      </c>
+      <c r="E39" t="s"/>
       <c r="F39" t="s"/>
       <c r="G39" t="s"/>
       <c r="H39" t="s"/>
       <c r="I39" t="s"/>
       <c r="J39" t="s"/>
-      <c r="K39" t="s"/>
+      <c r="K39" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B40" t="s"/>
       <c r="C40" t="s"/>
-      <c r="D40" t="s">
-        <v>18</v>
-      </c>
+      <c r="D40" t="s"/>
       <c r="E40" t="s"/>
       <c r="F40" t="s"/>
-      <c r="G40" t="s">
-        <v>18</v>
-      </c>
-      <c r="H40" t="s">
-        <v>24</v>
-      </c>
+      <c r="G40" t="s"/>
+      <c r="H40" t="s"/>
       <c r="I40" t="s"/>
-      <c r="J40" t="s"/>
+      <c r="J40" t="s">
+        <v>27</v>
+      </c>
       <c r="K40" t="s"/>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B41" t="s"/>
-      <c r="C41" t="s">
-        <v>31</v>
-      </c>
+      <c r="C41" t="s"/>
       <c r="D41" t="s"/>
       <c r="E41" t="s"/>
       <c r="F41" t="s"/>
       <c r="G41" t="s"/>
       <c r="H41" t="s"/>
-      <c r="I41" t="s"/>
+      <c r="I41" t="s">
+        <v>18</v>
+      </c>
       <c r="J41" t="s"/>
       <c r="K41" t="s"/>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" t="s"/>
-      <c r="D42" t="s"/>
+        <v>29</v>
+      </c>
+      <c r="C42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
       <c r="E42" t="s"/>
-      <c r="F42" t="s">
-        <v>46</v>
-      </c>
-      <c r="G42" t="s"/>
-      <c r="H42" t="s">
-        <v>102</v>
-      </c>
-      <c r="I42" t="s">
-        <v>40</v>
-      </c>
+      <c r="F42" t="s"/>
+      <c r="G42" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" t="s"/>
+      <c r="I42" t="s"/>
       <c r="J42" t="s"/>
       <c r="K42" t="s"/>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s"/>
-      <c r="E43" t="s"/>
+      <c r="E43" t="s">
+        <v>14</v>
+      </c>
       <c r="F43" t="s"/>
       <c r="G43" t="s"/>
-      <c r="H43" t="s">
-        <v>45</v>
-      </c>
+      <c r="H43" t="s"/>
       <c r="I43" t="s"/>
       <c r="J43" t="s"/>
       <c r="K43" t="s"/>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B44" t="s"/>
       <c r="C44" t="s"/>
@@ -1853,61 +1892,61 @@
       <c r="F44" t="s"/>
       <c r="G44" t="s"/>
       <c r="H44" t="s"/>
-      <c r="I44" t="s"/>
-      <c r="J44" t="s">
-        <v>55</v>
-      </c>
+      <c r="I44" t="s">
+        <v>18</v>
+      </c>
+      <c r="J44" t="s"/>
       <c r="K44" t="s"/>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B45" t="s"/>
       <c r="C45" t="s"/>
       <c r="D45" t="s"/>
-      <c r="E45" t="s"/>
-      <c r="F45" t="s"/>
+      <c r="E45" t="s">
+        <v>103</v>
+      </c>
+      <c r="F45" t="s">
+        <v>50</v>
+      </c>
       <c r="G45" t="s"/>
       <c r="H45" t="s"/>
-      <c r="I45" t="s">
-        <v>107</v>
-      </c>
-      <c r="J45" t="s">
-        <v>30</v>
-      </c>
-      <c r="K45" t="s"/>
+      <c r="I45" t="s"/>
+      <c r="J45" t="s"/>
+      <c r="K45" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B46" t="s"/>
-      <c r="C46" t="s">
-        <v>36</v>
-      </c>
-      <c r="D46" t="s"/>
+      <c r="C46" t="s"/>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
       <c r="E46" t="s"/>
       <c r="F46" t="s"/>
-      <c r="G46" t="s"/>
-      <c r="H46" t="s"/>
+      <c r="G46" t="s">
+        <v>20</v>
+      </c>
+      <c r="H46" t="s">
+        <v>26</v>
+      </c>
       <c r="I46" t="s"/>
-      <c r="J46" t="s">
-        <v>25</v>
-      </c>
-      <c r="K46" t="s">
-        <v>43</v>
-      </c>
+      <c r="J46" t="s"/>
+      <c r="K46" t="s"/>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B47" t="s">
-        <v>55</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B47" t="s"/>
       <c r="C47" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="D47" t="s"/>
       <c r="E47" t="s"/>
@@ -1920,72 +1959,70 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B48" t="s"/>
+        <v>106</v>
+      </c>
+      <c r="B48" t="s">
+        <v>107</v>
+      </c>
       <c r="C48" t="s"/>
-      <c r="D48" t="s">
-        <v>24</v>
-      </c>
+      <c r="D48" t="s"/>
       <c r="E48" t="s"/>
-      <c r="F48" t="s"/>
-      <c r="G48" t="s">
-        <v>24</v>
-      </c>
-      <c r="H48" t="s"/>
+      <c r="F48" t="s">
+        <v>47</v>
+      </c>
+      <c r="G48" t="s"/>
+      <c r="H48" t="s">
+        <v>108</v>
+      </c>
       <c r="I48" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="J48" t="s"/>
       <c r="K48" t="s"/>
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s"/>
       <c r="C49" t="s"/>
-      <c r="D49" t="s"/>
+      <c r="D49" t="s">
+        <v>46</v>
+      </c>
       <c r="E49" t="s"/>
       <c r="F49" t="s"/>
-      <c r="G49" t="s"/>
+      <c r="G49" t="s">
+        <v>46</v>
+      </c>
       <c r="H49" t="s"/>
       <c r="I49" t="s"/>
-      <c r="J49" t="s">
-        <v>30</v>
-      </c>
+      <c r="J49" t="s"/>
       <c r="K49" t="s"/>
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B50" t="s">
-        <v>113</v>
+        <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>76</v>
-      </c>
-      <c r="D50" t="s">
-        <v>37</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="D50" t="s"/>
       <c r="E50" t="s"/>
       <c r="F50" t="s"/>
-      <c r="G50" t="s">
-        <v>37</v>
-      </c>
-      <c r="H50" t="s"/>
-      <c r="I50" t="s">
-        <v>114</v>
-      </c>
-      <c r="J50" t="s">
-        <v>25</v>
-      </c>
+      <c r="G50" t="s"/>
+      <c r="H50" t="s">
+        <v>46</v>
+      </c>
+      <c r="I50" t="s"/>
+      <c r="J50" t="s"/>
       <c r="K50" t="s"/>
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B51" t="s"/>
       <c r="C51" t="s"/>
@@ -1996,152 +2033,156 @@
       <c r="H51" t="s"/>
       <c r="I51" t="s"/>
       <c r="J51" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K51" t="s"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B52" t="s"/>
-      <c r="C52" t="s">
-        <v>36</v>
-      </c>
+      <c r="C52" t="s"/>
       <c r="D52" t="s"/>
       <c r="E52" t="s"/>
-      <c r="F52" t="s">
+      <c r="F52" t="s"/>
+      <c r="G52" t="s"/>
+      <c r="H52" t="s"/>
+      <c r="I52" t="s">
+        <v>114</v>
+      </c>
+      <c r="J52" t="s">
         <v>32</v>
       </c>
-      <c r="G52" t="s"/>
-      <c r="H52" t="s">
-        <v>24</v>
-      </c>
-      <c r="I52" t="s"/>
-      <c r="J52" t="s">
-        <v>30</v>
-      </c>
-      <c r="K52" t="s">
-        <v>31</v>
-      </c>
+      <c r="K52" t="s"/>
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B53" t="s"/>
       <c r="C53" t="s"/>
-      <c r="D53" t="s">
-        <v>45</v>
-      </c>
+      <c r="D53" t="s"/>
       <c r="E53" t="s"/>
-      <c r="F53" t="s"/>
-      <c r="G53" t="s">
-        <v>45</v>
-      </c>
+      <c r="F53" t="s">
+        <v>50</v>
+      </c>
+      <c r="G53" t="s"/>
       <c r="H53" t="s"/>
       <c r="I53" t="s"/>
       <c r="J53" t="s"/>
-      <c r="K53" t="s"/>
+      <c r="K53" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B54" t="s"/>
-      <c r="C54" t="s"/>
+      <c r="C54" t="s">
+        <v>38</v>
+      </c>
       <c r="D54" t="s"/>
       <c r="E54" t="s"/>
       <c r="F54" t="s"/>
       <c r="G54" t="s"/>
-      <c r="H54" t="s">
-        <v>24</v>
-      </c>
+      <c r="H54" t="s"/>
       <c r="I54" t="s"/>
       <c r="J54" t="s">
-        <v>25</v>
-      </c>
-      <c r="K54" t="s"/>
+        <v>27</v>
+      </c>
+      <c r="K54" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B55" t="s"/>
-      <c r="C55" t="s"/>
+        <v>117</v>
+      </c>
+      <c r="B55" t="s">
+        <v>57</v>
+      </c>
+      <c r="C55" t="s">
+        <v>71</v>
+      </c>
       <c r="D55" t="s"/>
       <c r="E55" t="s"/>
       <c r="F55" t="s"/>
       <c r="G55" t="s"/>
-      <c r="H55" t="s">
-        <v>79</v>
-      </c>
-      <c r="I55" t="s">
-        <v>40</v>
-      </c>
+      <c r="H55" t="s"/>
+      <c r="I55" t="s"/>
       <c r="J55" t="s"/>
       <c r="K55" t="s"/>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B56" t="s">
-        <v>27</v>
-      </c>
-      <c r="C56" t="s">
-        <v>76</v>
-      </c>
-      <c r="D56" t="s"/>
+        <v>118</v>
+      </c>
+      <c r="B56" t="s"/>
+      <c r="C56" t="s"/>
+      <c r="D56" t="s">
+        <v>26</v>
+      </c>
       <c r="E56" t="s"/>
       <c r="F56" t="s"/>
-      <c r="G56" t="s"/>
+      <c r="G56" t="s">
+        <v>26</v>
+      </c>
       <c r="H56" t="s"/>
       <c r="I56" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J56" t="s"/>
       <c r="K56" t="s"/>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B57" t="s"/>
       <c r="C57" t="s"/>
-      <c r="D57" t="s">
-        <v>15</v>
-      </c>
+      <c r="D57" t="s"/>
       <c r="E57" t="s"/>
       <c r="F57" t="s"/>
-      <c r="G57" t="s">
-        <v>15</v>
-      </c>
+      <c r="G57" t="s"/>
       <c r="H57" t="s"/>
       <c r="I57" t="s"/>
-      <c r="J57" t="s"/>
+      <c r="J57" t="s">
+        <v>32</v>
+      </c>
       <c r="K57" t="s"/>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B58" t="s"/>
-      <c r="C58" t="s"/>
-      <c r="D58" t="s"/>
+        <v>120</v>
+      </c>
+      <c r="B58" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" t="s">
+        <v>78</v>
+      </c>
+      <c r="D58" t="s">
+        <v>39</v>
+      </c>
       <c r="E58" t="s"/>
       <c r="F58" t="s"/>
-      <c r="G58" t="s"/>
+      <c r="G58" t="s">
+        <v>39</v>
+      </c>
       <c r="H58" t="s"/>
       <c r="I58" t="s">
-        <v>123</v>
-      </c>
-      <c r="J58" t="s"/>
+        <v>122</v>
+      </c>
+      <c r="J58" t="s">
+        <v>27</v>
+      </c>
       <c r="K58" t="s"/>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B59" t="s"/>
       <c r="C59" t="s"/>
@@ -2151,50 +2192,58 @@
       <c r="G59" t="s"/>
       <c r="H59" t="s"/>
       <c r="I59" t="s"/>
-      <c r="J59" t="s"/>
-      <c r="K59" t="s">
-        <v>31</v>
-      </c>
+      <c r="J59" t="s">
+        <v>57</v>
+      </c>
+      <c r="K59" t="s"/>
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B60" t="s">
-        <v>113</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="B60" t="s"/>
       <c r="C60" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="D60" t="s"/>
       <c r="E60" t="s"/>
-      <c r="F60" t="s"/>
+      <c r="F60" t="s">
+        <v>34</v>
+      </c>
       <c r="G60" t="s"/>
-      <c r="H60" t="s"/>
+      <c r="H60" t="s">
+        <v>26</v>
+      </c>
       <c r="I60" t="s"/>
-      <c r="J60" t="s"/>
-      <c r="K60" t="s"/>
+      <c r="J60" t="s">
+        <v>32</v>
+      </c>
+      <c r="K60" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B61" t="s"/>
       <c r="C61" t="s"/>
-      <c r="D61" t="s"/>
+      <c r="D61" t="s">
+        <v>46</v>
+      </c>
       <c r="E61" t="s"/>
       <c r="F61" t="s"/>
-      <c r="G61" t="s"/>
-      <c r="H61" t="s">
-        <v>45</v>
-      </c>
+      <c r="G61" t="s">
+        <v>46</v>
+      </c>
+      <c r="H61" t="s"/>
       <c r="I61" t="s"/>
       <c r="J61" t="s"/>
       <c r="K61" t="s"/>
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s"/>
       <c r="C62" t="s"/>
@@ -2202,78 +2251,88 @@
       <c r="E62" t="s"/>
       <c r="F62" t="s"/>
       <c r="G62" t="s"/>
-      <c r="H62" t="s"/>
-      <c r="I62" t="s">
-        <v>107</v>
-      </c>
-      <c r="J62" t="s"/>
+      <c r="H62" t="s">
+        <v>26</v>
+      </c>
+      <c r="I62" t="s"/>
+      <c r="J62" t="s">
+        <v>27</v>
+      </c>
       <c r="K62" t="s"/>
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B63" t="s"/>
       <c r="C63" t="s"/>
       <c r="D63" t="s"/>
       <c r="E63" t="s"/>
       <c r="F63" t="s"/>
-      <c r="G63" t="s">
-        <v>45</v>
-      </c>
-      <c r="H63" t="s"/>
-      <c r="I63" t="s"/>
+      <c r="G63" t="s"/>
+      <c r="H63" t="s">
+        <v>81</v>
+      </c>
+      <c r="I63" t="s">
+        <v>18</v>
+      </c>
       <c r="J63" t="s"/>
       <c r="K63" t="s"/>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B64" t="s"/>
-      <c r="C64" t="s"/>
+        <v>128</v>
+      </c>
+      <c r="B64" t="s">
+        <v>29</v>
+      </c>
+      <c r="C64" t="s">
+        <v>78</v>
+      </c>
       <c r="D64" t="s"/>
       <c r="E64" t="s"/>
       <c r="F64" t="s"/>
       <c r="G64" t="s"/>
       <c r="H64" t="s"/>
-      <c r="I64" t="s"/>
-      <c r="J64" t="s">
-        <v>25</v>
-      </c>
+      <c r="I64" t="s">
+        <v>24</v>
+      </c>
+      <c r="J64" t="s"/>
       <c r="K64" t="s"/>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B65" t="s"/>
       <c r="C65" t="s"/>
-      <c r="D65" t="s"/>
+      <c r="D65" t="s">
+        <v>15</v>
+      </c>
       <c r="E65" t="s"/>
       <c r="F65" t="s"/>
-      <c r="G65" t="s"/>
+      <c r="G65" t="s">
+        <v>15</v>
+      </c>
       <c r="H65" t="s"/>
-      <c r="I65" t="s">
-        <v>22</v>
-      </c>
+      <c r="I65" t="s"/>
       <c r="J65" t="s"/>
       <c r="K65" t="s"/>
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B66" t="s"/>
       <c r="C66" t="s"/>
       <c r="D66" t="s"/>
       <c r="E66" t="s"/>
-      <c r="F66" t="s">
-        <v>46</v>
-      </c>
+      <c r="F66" t="s"/>
       <c r="G66" t="s"/>
       <c r="H66" t="s"/>
-      <c r="I66" t="s"/>
+      <c r="I66" t="s">
+        <v>131</v>
+      </c>
       <c r="J66" t="s"/>
       <c r="K66" t="s"/>
     </row>
@@ -2291,25 +2350,25 @@
       <c r="I67" t="s"/>
       <c r="J67" t="s"/>
       <c r="K67" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B68" t="s"/>
-      <c r="C68" t="s"/>
+      <c r="B68" t="s">
+        <v>121</v>
+      </c>
+      <c r="C68" t="s">
+        <v>78</v>
+      </c>
       <c r="D68" t="s"/>
       <c r="E68" t="s"/>
       <c r="F68" t="s"/>
-      <c r="G68" t="s">
-        <v>24</v>
-      </c>
+      <c r="G68" t="s"/>
       <c r="H68" t="s"/>
-      <c r="I68" t="s">
-        <v>40</v>
-      </c>
+      <c r="I68" t="s"/>
       <c r="J68" t="s"/>
       <c r="K68" t="s"/>
     </row>
@@ -2317,17 +2376,15 @@
       <c r="A69" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B69" t="s">
-        <v>25</v>
-      </c>
-      <c r="C69" t="s">
-        <v>43</v>
-      </c>
+      <c r="B69" t="s"/>
+      <c r="C69" t="s"/>
       <c r="D69" t="s"/>
       <c r="E69" t="s"/>
       <c r="F69" t="s"/>
       <c r="G69" t="s"/>
-      <c r="H69" t="s"/>
+      <c r="H69" t="s">
+        <v>46</v>
+      </c>
       <c r="I69" t="s"/>
       <c r="J69" t="s"/>
       <c r="K69" t="s"/>
@@ -2336,52 +2393,54 @@
       <c r="A70" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B70" t="s"/>
-      <c r="C70" t="s"/>
+      <c r="B70" t="s">
+        <v>69</v>
+      </c>
+      <c r="C70" t="s">
+        <v>136</v>
+      </c>
       <c r="D70" t="s"/>
       <c r="E70" t="s"/>
       <c r="F70" t="s"/>
       <c r="G70" t="s"/>
       <c r="H70" t="s"/>
       <c r="I70" t="s"/>
-      <c r="J70" t="s">
-        <v>16</v>
-      </c>
+      <c r="J70" t="s"/>
       <c r="K70" t="s"/>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B71" t="s">
-        <v>28</v>
-      </c>
-      <c r="C71" t="s">
-        <v>63</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="B71" t="s"/>
+      <c r="C71" t="s"/>
       <c r="D71" t="s"/>
       <c r="E71" t="s"/>
       <c r="F71" t="s"/>
       <c r="G71" t="s"/>
       <c r="H71" t="s"/>
-      <c r="I71" t="s"/>
+      <c r="I71" t="s">
+        <v>114</v>
+      </c>
       <c r="J71" t="s"/>
       <c r="K71" t="s"/>
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B72" t="s"/>
+        <v>138</v>
+      </c>
+      <c r="B72" t="s">
+        <v>139</v>
+      </c>
       <c r="C72" t="s">
-        <v>138</v>
+        <v>73</v>
       </c>
       <c r="D72" t="s"/>
       <c r="E72" t="s"/>
       <c r="F72" t="s"/>
       <c r="G72" t="s"/>
       <c r="H72" t="s">
-        <v>37</v>
+        <v>140</v>
       </c>
       <c r="I72" t="s"/>
       <c r="J72" t="s"/>
@@ -2389,28 +2448,24 @@
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B73" t="s">
-        <v>27</v>
-      </c>
-      <c r="C73" t="s">
-        <v>63</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="B73" t="s"/>
+      <c r="C73" t="s"/>
       <c r="D73" t="s"/>
       <c r="E73" t="s"/>
       <c r="F73" t="s"/>
-      <c r="G73" t="s"/>
+      <c r="G73" t="s">
+        <v>46</v>
+      </c>
       <c r="H73" t="s"/>
       <c r="I73" t="s"/>
-      <c r="J73" t="s">
-        <v>25</v>
-      </c>
+      <c r="J73" t="s"/>
       <c r="K73" t="s"/>
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B74" t="s"/>
       <c r="C74" t="s"/>
@@ -2419,76 +2474,62 @@
       <c r="F74" t="s"/>
       <c r="G74" t="s"/>
       <c r="H74" t="s"/>
-      <c r="I74" t="s">
-        <v>114</v>
-      </c>
-      <c r="J74" t="s"/>
+      <c r="I74" t="s"/>
+      <c r="J74" t="s">
+        <v>27</v>
+      </c>
       <c r="K74" t="s"/>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B75" t="s"/>
       <c r="C75" t="s"/>
-      <c r="D75" t="s">
-        <v>24</v>
-      </c>
+      <c r="D75" t="s"/>
       <c r="E75" t="s"/>
       <c r="F75" t="s"/>
-      <c r="G75" t="s">
+      <c r="G75" t="s"/>
+      <c r="H75" t="s"/>
+      <c r="I75" t="s">
         <v>24</v>
       </c>
-      <c r="H75" t="s"/>
-      <c r="I75" t="s"/>
       <c r="J75" t="s"/>
       <c r="K75" t="s"/>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B76" t="s"/>
       <c r="C76" t="s"/>
-      <c r="D76" t="s">
-        <v>24</v>
-      </c>
+      <c r="D76" t="s"/>
       <c r="E76" t="s"/>
       <c r="F76" t="s">
-        <v>32</v>
-      </c>
-      <c r="G76" t="s">
-        <v>24</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G76" t="s"/>
       <c r="H76" t="s"/>
       <c r="I76" t="s"/>
-      <c r="J76" t="s">
-        <v>30</v>
-      </c>
-      <c r="K76" t="s">
-        <v>31</v>
-      </c>
+      <c r="J76" t="s"/>
+      <c r="K76" t="s"/>
     </row>
     <row r="77" spans="1:11">
       <c r="A77" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B77" t="s">
-        <v>144</v>
-      </c>
-      <c r="C77" t="s">
         <v>145</v>
       </c>
+      <c r="B77" t="s"/>
+      <c r="C77" t="s"/>
       <c r="D77" t="s"/>
       <c r="E77" t="s"/>
       <c r="F77" t="s"/>
       <c r="G77" t="s"/>
-      <c r="H77" t="s">
-        <v>24</v>
-      </c>
+      <c r="H77" t="s"/>
       <c r="I77" t="s"/>
       <c r="J77" t="s"/>
-      <c r="K77" t="s"/>
+      <c r="K77" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="78" spans="1:11">
       <c r="A78" s="1" t="s">
@@ -2496,60 +2537,50 @@
       </c>
       <c r="B78" t="s"/>
       <c r="C78" t="s"/>
-      <c r="D78" t="s">
-        <v>147</v>
-      </c>
-      <c r="E78" t="s">
-        <v>20</v>
-      </c>
-      <c r="F78" t="s">
-        <v>148</v>
-      </c>
+      <c r="D78" t="s"/>
+      <c r="E78" t="s"/>
+      <c r="F78" t="s"/>
       <c r="G78" t="s">
-        <v>147</v>
-      </c>
-      <c r="H78" t="s">
-        <v>147</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="H78" t="s"/>
       <c r="I78" t="s">
-        <v>149</v>
-      </c>
-      <c r="J78" t="s">
-        <v>150</v>
-      </c>
-      <c r="K78" t="s">
-        <v>13</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="J78" t="s"/>
+      <c r="K78" t="s"/>
     </row>
     <row r="79" spans="1:11">
       <c r="A79" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B79" t="s"/>
       <c r="C79" t="s"/>
       <c r="D79" t="s"/>
       <c r="E79" t="s"/>
       <c r="F79" t="s"/>
-      <c r="G79" t="s"/>
-      <c r="H79" t="s">
+      <c r="G79" t="s">
         <v>15</v>
       </c>
+      <c r="H79" t="s"/>
       <c r="I79" t="s"/>
       <c r="J79" t="s"/>
       <c r="K79" t="s"/>
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B80" t="s"/>
-      <c r="C80" t="s"/>
+        <v>148</v>
+      </c>
+      <c r="B80" t="s">
+        <v>27</v>
+      </c>
+      <c r="C80" t="s">
+        <v>44</v>
+      </c>
       <c r="D80" t="s"/>
       <c r="E80" t="s"/>
       <c r="F80" t="s"/>
-      <c r="G80" t="s">
-        <v>45</v>
-      </c>
+      <c r="G80" t="s"/>
       <c r="H80" t="s"/>
       <c r="I80" t="s"/>
       <c r="J80" t="s"/>
@@ -2557,239 +2588,261 @@
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B81" t="s"/>
       <c r="C81" t="s"/>
       <c r="D81" t="s"/>
-      <c r="E81" t="s">
-        <v>20</v>
-      </c>
+      <c r="E81" t="s"/>
       <c r="F81" t="s"/>
       <c r="G81" t="s"/>
       <c r="H81" t="s"/>
       <c r="I81" t="s"/>
-      <c r="J81" t="s"/>
+      <c r="J81" t="s">
+        <v>16</v>
+      </c>
       <c r="K81" t="s"/>
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B82" t="s"/>
-      <c r="C82" t="s"/>
+        <v>150</v>
+      </c>
+      <c r="B82" t="s">
+        <v>30</v>
+      </c>
+      <c r="C82" t="s">
+        <v>65</v>
+      </c>
       <c r="D82" t="s"/>
       <c r="E82" t="s"/>
       <c r="F82" t="s"/>
       <c r="G82" t="s"/>
       <c r="H82" t="s"/>
-      <c r="I82" t="s">
-        <v>40</v>
-      </c>
+      <c r="I82" t="s"/>
       <c r="J82" t="s"/>
       <c r="K82" t="s"/>
     </row>
     <row r="83" spans="1:11">
       <c r="A83" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B83" t="s"/>
-      <c r="C83" t="s"/>
+      <c r="C83" t="s">
+        <v>136</v>
+      </c>
       <c r="D83" t="s"/>
       <c r="E83" t="s"/>
       <c r="F83" t="s"/>
       <c r="G83" t="s"/>
-      <c r="H83" t="s"/>
+      <c r="H83" t="s">
+        <v>39</v>
+      </c>
       <c r="I83" t="s"/>
-      <c r="J83" t="s">
-        <v>25</v>
-      </c>
+      <c r="J83" t="s"/>
       <c r="K83" t="s"/>
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B84" t="s"/>
-      <c r="C84" t="s"/>
-      <c r="D84" t="s">
-        <v>24</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="B84" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" t="s">
+        <v>65</v>
+      </c>
+      <c r="D84" t="s"/>
       <c r="E84" t="s"/>
       <c r="F84" t="s"/>
-      <c r="G84" t="s">
-        <v>24</v>
-      </c>
+      <c r="G84" t="s"/>
       <c r="H84" t="s"/>
       <c r="I84" t="s"/>
       <c r="J84" t="s">
-        <v>157</v>
+        <v>27</v>
       </c>
       <c r="K84" t="s"/>
     </row>
     <row r="85" spans="1:11">
       <c r="A85" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B85" t="s">
-        <v>28</v>
-      </c>
-      <c r="C85" t="s">
-        <v>28</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="B85" t="s"/>
+      <c r="C85" t="s"/>
       <c r="D85" t="s"/>
       <c r="E85" t="s"/>
       <c r="F85" t="s"/>
       <c r="G85" t="s"/>
-      <c r="H85" t="s">
-        <v>37</v>
-      </c>
-      <c r="I85" t="s"/>
+      <c r="H85" t="s"/>
+      <c r="I85" t="s">
+        <v>122</v>
+      </c>
       <c r="J85" t="s"/>
       <c r="K85" t="s"/>
     </row>
     <row r="86" spans="1:11">
       <c r="A86" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B86" t="s"/>
-      <c r="C86" t="s">
-        <v>65</v>
-      </c>
+      <c r="C86" t="s"/>
       <c r="D86" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="E86" t="s"/>
       <c r="F86" t="s"/>
-      <c r="G86" t="s"/>
-      <c r="H86" t="s">
-        <v>45</v>
-      </c>
+      <c r="G86" t="s">
+        <v>26</v>
+      </c>
+      <c r="H86" t="s"/>
       <c r="I86" t="s"/>
       <c r="J86" t="s"/>
       <c r="K86" t="s"/>
     </row>
     <row r="87" spans="1:11">
       <c r="A87" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B87" t="s">
-        <v>28</v>
-      </c>
-      <c r="C87" t="s">
-        <v>28</v>
-      </c>
-      <c r="D87" t="s"/>
+        <v>155</v>
+      </c>
+      <c r="B87" t="s"/>
+      <c r="C87" t="s"/>
+      <c r="D87" t="s">
+        <v>26</v>
+      </c>
       <c r="E87" t="s"/>
-      <c r="F87" t="s"/>
-      <c r="G87" t="s"/>
-      <c r="H87" t="s">
-        <v>21</v>
-      </c>
+      <c r="F87" t="s">
+        <v>34</v>
+      </c>
+      <c r="G87" t="s">
+        <v>26</v>
+      </c>
+      <c r="H87" t="s"/>
       <c r="I87" t="s"/>
-      <c r="J87" t="s"/>
-      <c r="K87" t="s"/>
+      <c r="J87" t="s">
+        <v>32</v>
+      </c>
+      <c r="K87" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="88" spans="1:11">
       <c r="A88" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B88" t="s"/>
-      <c r="C88" t="s"/>
+        <v>156</v>
+      </c>
+      <c r="B88" t="s">
+        <v>157</v>
+      </c>
+      <c r="C88" t="s">
+        <v>158</v>
+      </c>
       <c r="D88" t="s"/>
       <c r="E88" t="s"/>
       <c r="F88" t="s"/>
       <c r="G88" t="s"/>
-      <c r="H88" t="s"/>
+      <c r="H88" t="s">
+        <v>26</v>
+      </c>
       <c r="I88" t="s"/>
-      <c r="J88" t="s">
-        <v>42</v>
-      </c>
+      <c r="J88" t="s"/>
       <c r="K88" t="s"/>
     </row>
     <row r="89" spans="1:11">
       <c r="A89" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B89" t="s">
-        <v>113</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="B89" t="s"/>
       <c r="C89" t="s">
-        <v>76</v>
-      </c>
-      <c r="D89" t="s"/>
+        <v>38</v>
+      </c>
+      <c r="D89" t="s">
+        <v>26</v>
+      </c>
       <c r="E89" t="s"/>
-      <c r="F89" t="s"/>
-      <c r="G89" t="s"/>
+      <c r="F89" t="s">
+        <v>34</v>
+      </c>
+      <c r="G89" t="s">
+        <v>26</v>
+      </c>
       <c r="H89" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I89" t="s">
-        <v>114</v>
-      </c>
-      <c r="J89" t="s"/>
-      <c r="K89" t="s"/>
+        <v>122</v>
+      </c>
+      <c r="J89" t="s">
+        <v>32</v>
+      </c>
+      <c r="K89" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="90" spans="1:11">
       <c r="A90" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B90" t="s"/>
       <c r="C90" t="s"/>
       <c r="D90" t="s">
-        <v>24</v>
-      </c>
-      <c r="E90" t="s"/>
-      <c r="F90" t="s"/>
+        <v>161</v>
+      </c>
+      <c r="E90" t="s">
+        <v>22</v>
+      </c>
+      <c r="F90" t="s">
+        <v>162</v>
+      </c>
       <c r="G90" t="s">
-        <v>24</v>
+        <v>161</v>
       </c>
       <c r="H90" t="s">
-        <v>54</v>
+        <v>161</v>
       </c>
       <c r="I90" t="s">
-        <v>40</v>
-      </c>
-      <c r="J90" t="s"/>
-      <c r="K90" t="s"/>
+        <v>163</v>
+      </c>
+      <c r="J90" t="s">
+        <v>164</v>
+      </c>
+      <c r="K90" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="91" spans="1:11">
       <c r="A91" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B91" t="s"/>
-      <c r="C91" t="s">
-        <v>165</v>
-      </c>
+      <c r="C91" t="s"/>
       <c r="D91" t="s"/>
       <c r="E91" t="s"/>
-      <c r="F91" t="s"/>
+      <c r="F91" t="s">
+        <v>34</v>
+      </c>
       <c r="G91" t="s"/>
-      <c r="H91" t="s"/>
-      <c r="I91" t="s"/>
-      <c r="J91" t="s"/>
+      <c r="H91" t="s">
+        <v>26</v>
+      </c>
+      <c r="I91" t="s">
+        <v>18</v>
+      </c>
+      <c r="J91" t="s">
+        <v>32</v>
+      </c>
       <c r="K91" t="s"/>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B92" t="s">
-        <v>75</v>
-      </c>
-      <c r="C92" t="s">
-        <v>104</v>
-      </c>
+      <c r="B92" t="s"/>
+      <c r="C92" t="s"/>
       <c r="D92" t="s"/>
       <c r="E92" t="s"/>
       <c r="F92" t="s"/>
       <c r="G92" t="s"/>
       <c r="H92" t="s">
-        <v>45</v>
-      </c>
-      <c r="I92" t="s">
-        <v>107</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="I92" t="s"/>
       <c r="J92" t="s"/>
       <c r="K92" t="s"/>
     </row>
@@ -2797,198 +2850,176 @@
       <c r="A93" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B93" t="s">
-        <v>25</v>
-      </c>
-      <c r="C93" t="s">
-        <v>69</v>
-      </c>
-      <c r="D93" t="s">
-        <v>168</v>
-      </c>
+      <c r="B93" t="s"/>
+      <c r="C93" t="s"/>
+      <c r="D93" t="s"/>
       <c r="E93" t="s"/>
       <c r="F93" t="s"/>
       <c r="G93" t="s">
-        <v>45</v>
-      </c>
-      <c r="H93" t="s">
-        <v>45</v>
-      </c>
-      <c r="I93" t="s">
-        <v>107</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="H93" t="s"/>
+      <c r="I93" t="s"/>
       <c r="J93" t="s"/>
       <c r="K93" t="s"/>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B94" t="s">
-        <v>75</v>
-      </c>
-      <c r="C94" t="s">
-        <v>76</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="B94" t="s"/>
+      <c r="C94" t="s"/>
       <c r="D94" t="s"/>
-      <c r="E94" t="s"/>
+      <c r="E94" t="s">
+        <v>22</v>
+      </c>
       <c r="F94" t="s"/>
       <c r="G94" t="s"/>
       <c r="H94" t="s"/>
-      <c r="I94" t="s">
-        <v>40</v>
-      </c>
-      <c r="J94" t="s">
-        <v>30</v>
-      </c>
+      <c r="I94" t="s"/>
+      <c r="J94" t="s"/>
       <c r="K94" t="s"/>
     </row>
     <row r="95" spans="1:11">
       <c r="A95" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B95" t="s"/>
       <c r="C95" t="s"/>
-      <c r="D95" t="s">
-        <v>54</v>
-      </c>
+      <c r="D95" t="s"/>
       <c r="E95" t="s"/>
       <c r="F95" t="s"/>
-      <c r="G95" t="s">
-        <v>54</v>
-      </c>
+      <c r="G95" t="s"/>
       <c r="H95" t="s"/>
-      <c r="I95" t="s"/>
+      <c r="I95" t="s">
+        <v>18</v>
+      </c>
       <c r="J95" t="s"/>
-      <c r="K95" t="s">
-        <v>71</v>
-      </c>
+      <c r="K95" t="s"/>
     </row>
     <row r="96" spans="1:11">
       <c r="A96" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B96" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C96" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D96" t="s"/>
       <c r="E96" t="s"/>
       <c r="F96" t="s"/>
       <c r="G96" t="s"/>
       <c r="H96" t="s"/>
-      <c r="I96" t="s">
-        <v>114</v>
-      </c>
+      <c r="I96" t="s"/>
       <c r="J96" t="s"/>
       <c r="K96" t="s"/>
     </row>
     <row r="97" spans="1:11">
       <c r="A97" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B97" t="s">
-        <v>67</v>
-      </c>
-      <c r="C97" t="s">
-        <v>65</v>
-      </c>
-      <c r="D97" t="s">
-        <v>24</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="B97" t="s"/>
+      <c r="C97" t="s"/>
+      <c r="D97" t="s"/>
       <c r="E97" t="s"/>
-      <c r="F97" t="s">
-        <v>32</v>
-      </c>
-      <c r="G97" t="s">
-        <v>24</v>
-      </c>
-      <c r="H97" t="s">
-        <v>24</v>
-      </c>
+      <c r="F97" t="s"/>
+      <c r="G97" t="s"/>
+      <c r="H97" t="s"/>
       <c r="I97" t="s"/>
-      <c r="J97" t="s"/>
-      <c r="K97" t="s">
-        <v>31</v>
-      </c>
+      <c r="J97" t="s">
+        <v>27</v>
+      </c>
+      <c r="K97" t="s"/>
     </row>
     <row r="98" spans="1:11">
       <c r="A98" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B98" t="s"/>
       <c r="C98" t="s"/>
       <c r="D98" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E98" t="s"/>
       <c r="F98" t="s"/>
-      <c r="G98" t="s"/>
+      <c r="G98" t="s">
+        <v>26</v>
+      </c>
       <c r="H98" t="s"/>
       <c r="I98" t="s"/>
-      <c r="J98" t="s"/>
+      <c r="J98" t="s">
+        <v>139</v>
+      </c>
       <c r="K98" t="s"/>
     </row>
     <row r="99" spans="1:11">
       <c r="A99" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B99" t="s"/>
-      <c r="C99" t="s"/>
-      <c r="D99" t="s">
-        <v>24</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="B99" t="s">
+        <v>30</v>
+      </c>
+      <c r="C99" t="s">
+        <v>30</v>
+      </c>
+      <c r="D99" t="s"/>
       <c r="E99" t="s"/>
-      <c r="F99" t="s">
-        <v>46</v>
-      </c>
-      <c r="G99" t="s">
-        <v>24</v>
-      </c>
-      <c r="H99" t="s"/>
+      <c r="F99" t="s"/>
+      <c r="G99" t="s"/>
+      <c r="H99" t="s">
+        <v>39</v>
+      </c>
       <c r="I99" t="s"/>
       <c r="J99" t="s"/>
       <c r="K99" t="s"/>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B100" t="s"/>
-      <c r="C100" t="s"/>
-      <c r="D100" t="s"/>
+      <c r="C100" t="s">
+        <v>67</v>
+      </c>
+      <c r="D100" t="s">
+        <v>74</v>
+      </c>
       <c r="E100" t="s"/>
-      <c r="F100" t="s">
-        <v>176</v>
-      </c>
+      <c r="F100" t="s"/>
       <c r="G100" t="s"/>
-      <c r="H100" t="s"/>
+      <c r="H100" t="s">
+        <v>46</v>
+      </c>
       <c r="I100" t="s"/>
       <c r="J100" t="s"/>
       <c r="K100" t="s"/>
     </row>
     <row r="101" spans="1:11">
       <c r="A101" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B101" t="s"/>
-      <c r="C101" t="s"/>
+        <v>175</v>
+      </c>
+      <c r="B101" t="s">
+        <v>30</v>
+      </c>
+      <c r="C101" t="s">
+        <v>30</v>
+      </c>
       <c r="D101" t="s"/>
       <c r="E101" t="s"/>
       <c r="F101" t="s"/>
       <c r="G101" t="s"/>
-      <c r="H101" t="s"/>
-      <c r="I101" t="s">
-        <v>40</v>
-      </c>
+      <c r="H101" t="s">
+        <v>23</v>
+      </c>
+      <c r="I101" t="s"/>
       <c r="J101" t="s"/>
       <c r="K101" t="s"/>
     </row>
     <row r="102" spans="1:11">
       <c r="A102" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B102" t="s"/>
       <c r="C102" t="s"/>
@@ -2999,57 +3030,67 @@
       <c r="H102" t="s"/>
       <c r="I102" t="s"/>
       <c r="J102" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="K102" t="s"/>
     </row>
     <row r="103" spans="1:11">
       <c r="A103" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B103" t="s"/>
-      <c r="C103" t="s"/>
-      <c r="D103" t="s">
-        <v>37</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="B103" t="s">
+        <v>121</v>
+      </c>
+      <c r="C103" t="s">
+        <v>78</v>
+      </c>
+      <c r="D103" t="s"/>
       <c r="E103" t="s"/>
       <c r="F103" t="s"/>
       <c r="G103" t="s"/>
-      <c r="H103" t="s"/>
-      <c r="I103" t="s"/>
+      <c r="H103" t="s">
+        <v>20</v>
+      </c>
+      <c r="I103" t="s">
+        <v>122</v>
+      </c>
       <c r="J103" t="s"/>
       <c r="K103" t="s"/>
     </row>
     <row r="104" spans="1:11">
       <c r="A104" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B104" t="s"/>
       <c r="C104" t="s"/>
-      <c r="D104" t="s"/>
+      <c r="D104" t="s">
+        <v>26</v>
+      </c>
       <c r="E104" t="s"/>
       <c r="F104" t="s"/>
       <c r="G104" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="H104" t="s">
-        <v>15</v>
-      </c>
-      <c r="I104" t="s"/>
+        <v>56</v>
+      </c>
+      <c r="I104" t="s">
+        <v>18</v>
+      </c>
       <c r="J104" t="s"/>
       <c r="K104" t="s"/>
     </row>
     <row r="105" spans="1:11">
       <c r="A105" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B105" t="s"/>
-      <c r="C105" t="s"/>
+      <c r="C105" t="s">
+        <v>180</v>
+      </c>
       <c r="D105" t="s"/>
       <c r="E105" t="s"/>
-      <c r="F105" t="s">
-        <v>46</v>
-      </c>
+      <c r="F105" t="s"/>
       <c r="G105" t="s"/>
       <c r="H105" t="s"/>
       <c r="I105" t="s"/>
@@ -3058,43 +3099,51 @@
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B106" t="s">
-        <v>25</v>
-      </c>
-      <c r="C106" t="s"/>
+        <v>77</v>
+      </c>
+      <c r="C106" t="s">
+        <v>111</v>
+      </c>
       <c r="D106" t="s"/>
       <c r="E106" t="s"/>
       <c r="F106" t="s"/>
       <c r="G106" t="s"/>
-      <c r="H106" t="s"/>
+      <c r="H106" t="s">
+        <v>46</v>
+      </c>
       <c r="I106" t="s">
-        <v>40</v>
-      </c>
-      <c r="J106" t="s">
-        <v>25</v>
-      </c>
-      <c r="K106" t="s">
-        <v>71</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="J106" t="s"/>
+      <c r="K106" t="s"/>
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B107" t="s">
+        <v>27</v>
+      </c>
+      <c r="C107" t="s">
+        <v>71</v>
+      </c>
+      <c r="D107" t="s">
         <v>183</v>
       </c>
-      <c r="B107" t="s">
-        <v>75</v>
-      </c>
-      <c r="C107" t="s">
-        <v>63</v>
-      </c>
-      <c r="D107" t="s"/>
       <c r="E107" t="s"/>
       <c r="F107" t="s"/>
-      <c r="G107" t="s"/>
-      <c r="H107" t="s"/>
-      <c r="I107" t="s"/>
+      <c r="G107" t="s">
+        <v>46</v>
+      </c>
+      <c r="H107" t="s">
+        <v>46</v>
+      </c>
+      <c r="I107" t="s">
+        <v>114</v>
+      </c>
       <c r="J107" t="s"/>
       <c r="K107" t="s"/>
     </row>
@@ -3102,17 +3151,23 @@
       <c r="A108" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B108" t="s"/>
-      <c r="C108" t="s"/>
+      <c r="B108" t="s">
+        <v>77</v>
+      </c>
+      <c r="C108" t="s">
+        <v>78</v>
+      </c>
       <c r="D108" t="s"/>
       <c r="E108" t="s"/>
       <c r="F108" t="s"/>
       <c r="G108" t="s"/>
-      <c r="H108" t="s">
-        <v>24</v>
-      </c>
-      <c r="I108" t="s"/>
-      <c r="J108" t="s"/>
+      <c r="H108" t="s"/>
+      <c r="I108" t="s">
+        <v>18</v>
+      </c>
+      <c r="J108" t="s">
+        <v>32</v>
+      </c>
       <c r="K108" t="s"/>
     </row>
     <row r="109" spans="1:11">
@@ -3121,43 +3176,37 @@
       </c>
       <c r="B109" t="s"/>
       <c r="C109" t="s"/>
-      <c r="D109" t="s"/>
+      <c r="D109" t="s">
+        <v>56</v>
+      </c>
       <c r="E109" t="s"/>
-      <c r="F109" t="s">
-        <v>32</v>
-      </c>
+      <c r="F109" t="s"/>
       <c r="G109" t="s">
-        <v>24</v>
-      </c>
-      <c r="H109" t="s">
-        <v>24</v>
-      </c>
-      <c r="I109" t="s">
-        <v>33</v>
-      </c>
-      <c r="J109" t="s">
-        <v>30</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="H109" t="s"/>
+      <c r="I109" t="s"/>
+      <c r="J109" t="s"/>
       <c r="K109" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B110" t="s"/>
+      <c r="B110" t="s">
+        <v>27</v>
+      </c>
       <c r="C110" t="s"/>
-      <c r="D110" t="s">
-        <v>24</v>
-      </c>
+      <c r="D110" t="s"/>
       <c r="E110" t="s"/>
       <c r="F110" t="s"/>
-      <c r="G110" t="s">
-        <v>24</v>
-      </c>
+      <c r="G110" t="s"/>
       <c r="H110" t="s"/>
-      <c r="I110" t="s"/>
+      <c r="I110" t="s">
+        <v>131</v>
+      </c>
       <c r="J110" t="s"/>
       <c r="K110" t="s"/>
     </row>
@@ -3166,49 +3215,365 @@
         <v>187</v>
       </c>
       <c r="B111" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C111" t="s">
-        <v>188</v>
+        <v>30</v>
       </c>
       <c r="D111" t="s"/>
       <c r="E111" t="s"/>
       <c r="F111" t="s"/>
       <c r="G111" t="s"/>
-      <c r="H111" t="s">
-        <v>15</v>
-      </c>
-      <c r="I111" t="s"/>
+      <c r="H111" t="s"/>
+      <c r="I111" t="s">
+        <v>122</v>
+      </c>
       <c r="J111" t="s"/>
       <c r="K111" t="s"/>
     </row>
     <row r="112" spans="1:11">
       <c r="A112" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B112" t="s"/>
-      <c r="C112" t="s"/>
+        <v>188</v>
+      </c>
+      <c r="B112" t="s">
+        <v>69</v>
+      </c>
+      <c r="C112" t="s">
+        <v>67</v>
+      </c>
       <c r="D112" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E112" t="s"/>
       <c r="F112" t="s">
+        <v>34</v>
+      </c>
+      <c r="G112" t="s">
+        <v>26</v>
+      </c>
+      <c r="H112" t="s">
+        <v>26</v>
+      </c>
+      <c r="I112" t="s"/>
+      <c r="J112" t="s"/>
+      <c r="K112" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
+      <c r="A113" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B113" t="s"/>
+      <c r="C113" t="s"/>
+      <c r="D113" t="s">
+        <v>26</v>
+      </c>
+      <c r="E113" t="s"/>
+      <c r="F113" t="s"/>
+      <c r="G113" t="s"/>
+      <c r="H113" t="s"/>
+      <c r="I113" t="s"/>
+      <c r="J113" t="s"/>
+      <c r="K113" t="s"/>
+    </row>
+    <row r="114" spans="1:11">
+      <c r="A114" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G112" t="s">
-        <v>24</v>
-      </c>
-      <c r="H112" t="s">
-        <v>37</v>
-      </c>
-      <c r="I112" t="s">
-        <v>40</v>
-      </c>
-      <c r="J112" t="s">
-        <v>55</v>
-      </c>
-      <c r="K112" t="s">
-        <v>90</v>
+      <c r="B114" t="s"/>
+      <c r="C114" t="s"/>
+      <c r="D114" t="s">
+        <v>26</v>
+      </c>
+      <c r="E114" t="s"/>
+      <c r="F114" t="s">
+        <v>47</v>
+      </c>
+      <c r="G114" t="s">
+        <v>26</v>
+      </c>
+      <c r="H114" t="s"/>
+      <c r="I114" t="s"/>
+      <c r="J114" t="s"/>
+      <c r="K114" t="s"/>
+    </row>
+    <row r="115" spans="1:11">
+      <c r="A115" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B115" t="s"/>
+      <c r="C115" t="s"/>
+      <c r="D115" t="s"/>
+      <c r="E115" t="s"/>
+      <c r="F115" t="s">
+        <v>192</v>
+      </c>
+      <c r="G115" t="s"/>
+      <c r="H115" t="s"/>
+      <c r="I115" t="s"/>
+      <c r="J115" t="s"/>
+      <c r="K115" t="s"/>
+    </row>
+    <row r="116" spans="1:11">
+      <c r="A116" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B116" t="s"/>
+      <c r="C116" t="s"/>
+      <c r="D116" t="s"/>
+      <c r="E116" t="s"/>
+      <c r="F116" t="s">
+        <v>50</v>
+      </c>
+      <c r="G116" t="s"/>
+      <c r="H116" t="s"/>
+      <c r="I116" t="s"/>
+      <c r="J116" t="s"/>
+      <c r="K116" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
+      <c r="A117" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B117" t="s"/>
+      <c r="C117" t="s"/>
+      <c r="D117" t="s"/>
+      <c r="E117" t="s"/>
+      <c r="F117" t="s"/>
+      <c r="G117" t="s"/>
+      <c r="H117" t="s"/>
+      <c r="I117" t="s">
+        <v>18</v>
+      </c>
+      <c r="J117" t="s"/>
+      <c r="K117" t="s"/>
+    </row>
+    <row r="118" spans="1:11">
+      <c r="A118" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B118" t="s"/>
+      <c r="C118" t="s"/>
+      <c r="D118" t="s"/>
+      <c r="E118" t="s"/>
+      <c r="F118" t="s"/>
+      <c r="G118" t="s"/>
+      <c r="H118" t="s"/>
+      <c r="I118" t="s"/>
+      <c r="J118" t="s">
+        <v>27</v>
+      </c>
+      <c r="K118" t="s"/>
+    </row>
+    <row r="119" spans="1:11">
+      <c r="A119" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B119" t="s"/>
+      <c r="C119" t="s"/>
+      <c r="D119" t="s">
+        <v>39</v>
+      </c>
+      <c r="E119" t="s"/>
+      <c r="F119" t="s"/>
+      <c r="G119" t="s"/>
+      <c r="H119" t="s"/>
+      <c r="I119" t="s"/>
+      <c r="J119" t="s"/>
+      <c r="K119" t="s"/>
+    </row>
+    <row r="120" spans="1:11">
+      <c r="A120" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B120" t="s"/>
+      <c r="C120" t="s"/>
+      <c r="D120" t="s"/>
+      <c r="E120" t="s"/>
+      <c r="F120" t="s"/>
+      <c r="G120" t="s">
+        <v>15</v>
+      </c>
+      <c r="H120" t="s">
+        <v>15</v>
+      </c>
+      <c r="I120" t="s"/>
+      <c r="J120" t="s"/>
+      <c r="K120" t="s"/>
+    </row>
+    <row r="121" spans="1:11">
+      <c r="A121" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B121" t="s"/>
+      <c r="C121" t="s"/>
+      <c r="D121" t="s"/>
+      <c r="E121" t="s"/>
+      <c r="F121" t="s">
+        <v>47</v>
+      </c>
+      <c r="G121" t="s"/>
+      <c r="H121" t="s"/>
+      <c r="I121" t="s"/>
+      <c r="J121" t="s"/>
+      <c r="K121" t="s"/>
+    </row>
+    <row r="122" spans="1:11">
+      <c r="A122" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B122" t="s">
+        <v>27</v>
+      </c>
+      <c r="C122" t="s"/>
+      <c r="D122" t="s"/>
+      <c r="E122" t="s"/>
+      <c r="F122" t="s"/>
+      <c r="G122" t="s"/>
+      <c r="H122" t="s"/>
+      <c r="I122" t="s">
+        <v>18</v>
+      </c>
+      <c r="J122" t="s">
+        <v>27</v>
+      </c>
+      <c r="K122" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
+      <c r="A123" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B123" t="s">
+        <v>77</v>
+      </c>
+      <c r="C123" t="s">
+        <v>65</v>
+      </c>
+      <c r="D123" t="s"/>
+      <c r="E123" t="s"/>
+      <c r="F123" t="s"/>
+      <c r="G123" t="s"/>
+      <c r="H123" t="s"/>
+      <c r="I123" t="s"/>
+      <c r="J123" t="s"/>
+      <c r="K123" t="s"/>
+    </row>
+    <row r="124" spans="1:11">
+      <c r="A124" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B124" t="s"/>
+      <c r="C124" t="s"/>
+      <c r="D124" t="s"/>
+      <c r="E124" t="s"/>
+      <c r="F124" t="s"/>
+      <c r="G124" t="s"/>
+      <c r="H124" t="s">
+        <v>26</v>
+      </c>
+      <c r="I124" t="s"/>
+      <c r="J124" t="s"/>
+      <c r="K124" t="s"/>
+    </row>
+    <row r="125" spans="1:11">
+      <c r="A125" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B125" t="s"/>
+      <c r="C125" t="s"/>
+      <c r="D125" t="s"/>
+      <c r="E125" t="s"/>
+      <c r="F125" t="s">
+        <v>34</v>
+      </c>
+      <c r="G125" t="s">
+        <v>26</v>
+      </c>
+      <c r="H125" t="s">
+        <v>26</v>
+      </c>
+      <c r="I125" t="s">
+        <v>35</v>
+      </c>
+      <c r="J125" t="s">
+        <v>32</v>
+      </c>
+      <c r="K125" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
+      <c r="A126" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B126" t="s"/>
+      <c r="C126" t="s"/>
+      <c r="D126" t="s">
+        <v>26</v>
+      </c>
+      <c r="E126" t="s"/>
+      <c r="F126" t="s"/>
+      <c r="G126" t="s">
+        <v>26</v>
+      </c>
+      <c r="H126" t="s"/>
+      <c r="I126" t="s"/>
+      <c r="J126" t="s"/>
+      <c r="K126" t="s"/>
+    </row>
+    <row r="127" spans="1:11">
+      <c r="A127" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B127" t="s">
+        <v>43</v>
+      </c>
+      <c r="C127" t="s">
+        <v>205</v>
+      </c>
+      <c r="D127" t="s"/>
+      <c r="E127" t="s"/>
+      <c r="F127" t="s"/>
+      <c r="G127" t="s"/>
+      <c r="H127" t="s">
+        <v>15</v>
+      </c>
+      <c r="I127" t="s"/>
+      <c r="J127" t="s"/>
+      <c r="K127" t="s"/>
+    </row>
+    <row r="128" spans="1:11">
+      <c r="A128" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B128" t="s"/>
+      <c r="C128" t="s"/>
+      <c r="D128" t="s">
+        <v>26</v>
+      </c>
+      <c r="E128" t="s"/>
+      <c r="F128" t="s">
+        <v>207</v>
+      </c>
+      <c r="G128" t="s">
+        <v>26</v>
+      </c>
+      <c r="H128" t="s">
+        <v>39</v>
+      </c>
+      <c r="I128" t="s">
+        <v>18</v>
+      </c>
+      <c r="J128" t="s">
+        <v>57</v>
+      </c>
+      <c r="K128" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>